<commit_message>
Comitting all the files, mainly measurement and R scripts from the day prior.
</commit_message>
<xml_diff>
--- a/organ_measure.xlsx
+++ b/organ_measure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/435577af404d2ec7/2023/BME_M2/STAGE/Thesis/Scripts_and_venv/internship_M2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5490666-A945-4A55-88F2-1C034C3CA3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{B5490666-A945-4A55-88F2-1C034C3CA3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53715E4E-AB15-40B8-BF53-97776E5499CD}"/>
   <bookViews>
-    <workbookView xWindow="5484" yWindow="180" windowWidth="17628" windowHeight="10164" xr2:uid="{E7F36383-A453-45E0-8469-92D4BA6D15DB}"/>
+    <workbookView xWindow="51105" yWindow="2985" windowWidth="17625" windowHeight="10170" xr2:uid="{E7F36383-A453-45E0-8469-92D4BA6D15DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="26">
   <si>
     <t>t1</t>
   </si>
@@ -120,13 +120,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD6DEEB"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -161,10 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,18 +508,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1426DD-ABA7-4F24-B0C3-92136F16B0F8}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="1"/>
-    <col min="11" max="11" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" style="1"/>
+    <col min="11" max="11" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -547,7 +554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -560,31 +567,31 @@
       <c r="D2">
         <v>-549</v>
       </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
+      <c r="E2" s="3">
+        <v>-364.89473700000002</v>
+      </c>
+      <c r="F2" s="3">
+        <v>-479.78947399999998</v>
       </c>
       <c r="G2">
         <v>-365</v>
       </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
+      <c r="H2" s="3">
+        <v>-604.89473699999996</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-305.90476200000001</v>
       </c>
       <c r="J2" s="1">
         <f>AVERAGE(B2:I2)</f>
-        <v>-527.5</v>
+        <v>-483.18546375000005</v>
       </c>
       <c r="K2" s="2">
         <f>_xlfn.STDEV.S(B2:I2)</f>
-        <v>155.69307413412238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>141.83588891071605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -621,7 +628,7 @@
         <v>147.05424030408938</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -658,7 +665,7 @@
         <v>99.78479922279061</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -695,7 +702,7 @@
         <v>121.19404848679484</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -732,7 +739,7 @@
         <v>126.71350468343864</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -761,7 +768,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -774,31 +781,31 @@
       <c r="D9">
         <v>0.218</v>
       </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
+      <c r="E9" s="3">
+        <v>0.37052600000000002</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.86421099999999995</v>
       </c>
       <c r="G9">
         <v>1.65</v>
       </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>25</v>
+      <c r="H9" s="3">
+        <v>0.148421</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.9</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="0"/>
-        <v>0.87424999999999997</v>
+        <v>0.84751975000000002</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>0.7212980775426111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.69569350284626053</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -835,7 +842,7 @@
         <v>6.9070888418798881E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -872,7 +879,7 @@
         <v>0.12612412359326747</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -909,7 +916,7 @@
         <v>0.17406688504972495</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -946,7 +953,7 @@
         <v>8.4020108176697431E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -975,7 +982,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -988,31 +995,31 @@
       <c r="D16">
         <v>-533</v>
       </c>
-      <c r="E16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" t="s">
-        <v>25</v>
+      <c r="E16" s="3">
+        <v>-585.684211</v>
+      </c>
+      <c r="F16" s="3">
+        <v>-422.57894700000003</v>
       </c>
       <c r="G16">
         <v>-363</v>
       </c>
-      <c r="H16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" t="s">
-        <v>25</v>
+      <c r="H16" s="3">
+        <v>-652.95000000000005</v>
+      </c>
+      <c r="I16" s="3">
+        <v>-122.38888900000001</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="0"/>
-        <v>-501.25</v>
+        <v>-473.57525587499993</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="1"/>
-        <v>149.41748001265893</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+        <v>185.44021766611883</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1049,7 +1056,7 @@
         <v>107.27130632607769</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1086,7 +1093,7 @@
         <v>97.26586631739022</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +1130,7 @@
         <v>120.08366593132945</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1160,7 +1167,7 @@
         <v>131.13826278536825</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1189,7 +1196,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1202,31 +1209,31 @@
       <c r="D23">
         <v>0.24</v>
       </c>
-      <c r="E23" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" t="s">
-        <v>25</v>
+      <c r="E23" s="3">
+        <v>0.24315800000000001</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1.6926319999999999</v>
       </c>
       <c r="G23">
         <v>1.3640000000000001</v>
       </c>
-      <c r="H23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" t="s">
-        <v>25</v>
+      <c r="H23" s="3">
+        <v>0.223</v>
+      </c>
+      <c r="I23" s="3">
+        <v>2.605556</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="0"/>
-        <v>0.85349999999999993</v>
+        <v>1.0222932499999999</v>
       </c>
       <c r="K23" s="2">
         <f t="shared" si="1"/>
-        <v>0.87184612556727392</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.97073669061620416</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>0.14123019797784675</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1300,7 +1307,7 @@
         <v>0.2289764137084197</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1337,7 +1344,7 @@
         <v>0.16422190789907903</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1374,7 +1381,7 @@
         <v>0.10423140845223425</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1403,7 +1410,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1440,7 +1447,7 @@
         <v>7.846929665214387</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1477,7 +1484,7 @@
         <v>12.877112382202139</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1514,7 +1521,7 @@
         <v>11.143914873042663</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1551,7 +1558,7 @@
         <v>10.394156884187829</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1588,7 +1595,7 @@
         <v>11.947662893218027</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1617,7 +1624,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -1654,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -1691,7 +1698,7 @@
         <v>0.16002420670252476</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -1728,7 +1735,7 @@
         <v>0.16597694067644486</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1765,7 +1772,7 @@
         <v>0.12529681123033415</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1802,7 +1809,7 @@
         <v>6.2815978204550121E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -1831,7 +1838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -1868,7 +1875,7 @@
         <v>52.277931700260893</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -1905,7 +1912,7 @@
         <v>19.891217720116551</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -1942,7 +1949,7 @@
         <v>14.46367949665297</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1979,7 +1986,7 @@
         <v>18.28916973848818</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -2016,7 +2023,7 @@
         <v>9.6064243915701528</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -2045,7 +2052,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2082,7 +2089,7 @@
         <v>0.86876051894967832</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -2119,7 +2126,7 @@
         <v>0.26804918133575506</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -2156,7 +2163,7 @@
         <v>0.17600373020975152</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -2193,7 +2200,7 @@
         <v>0.23628504993832028</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>7.0839551086116309E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -2259,7 +2266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -2296,7 +2303,7 @@
         <v>45.943871035365376</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>1</v>
       </c>
@@ -2333,7 +2340,7 @@
         <v>23.966084034790054</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -2370,7 +2377,7 @@
         <v>16.954233345234062</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -2407,7 +2414,7 @@
         <v>21.02401168179339</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -2444,7 +2451,7 @@
         <v>16.65508335407289</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -2473,7 +2480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -2510,7 +2517,7 @@
         <v>0.63442093957515977</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -2547,7 +2554,7 @@
         <v>0.31193884442997022</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -2584,7 +2591,7 @@
         <v>0.18537657279959588</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -2621,7 +2628,7 @@
         <v>9.4274716271128059E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Life is going good. Finishing up abstracts and have a little script here for maximum intensity projections which are sooo easy to make! The gif on the other hand i mostly did thanks to GPT but I had to troubleshoot it. Kedge images are noisy but well see...
</commit_message>
<xml_diff>
--- a/organ_measure.xlsx
+++ b/organ_measure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/435577af404d2ec7/2023/BME_M2/STAGE/Thesis/Scripts_and_venv/internship_M2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="922" documentId="8_{B5490666-A945-4A55-88F2-1C034C3CA3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C98E9C50-8F81-47FE-98F1-31FEC8EB4D7F}"/>
+  <xr:revisionPtr revIDLastSave="998" documentId="8_{B5490666-A945-4A55-88F2-1C034C3CA3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C71921-D05A-4DED-9DE7-BCA590579ED0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{E7F36383-A453-45E0-8469-92D4BA6D15DB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{E7F36383-A453-45E0-8469-92D4BA6D15DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="92">
   <si>
     <t>t1</t>
   </si>
@@ -304,6 +304,18 @@
   <si>
     <t>statistics</t>
   </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>mg/mL</t>
+  </si>
+  <si>
+    <t>(From sample 6)</t>
+  </si>
+  <si>
+    <t>Conversion</t>
+  </si>
 </sst>
 </file>
 
@@ -456,6 +468,998 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3D Anal 2'!$AX$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mg/mL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.3882588070986536E-2"/>
+                  <c:y val="-0.15383542538354253"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'3D Anal 2'!$AW$41:$AW$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>83.39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>215.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>360.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>521.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'3D Anal 2'!$AX$41:$AX$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6736-4796-89B1-94AAEEBC495D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1406183999"/>
+        <c:axId val="1406181599"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1406183999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1406181599"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1406181599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1406183999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>35523</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>94576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>142650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4486321C-F794-6098-DBB7-45E4D41D12E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -781,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1426DD-ABA7-4F24-B0C3-92136F16B0F8}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6246,10 +7250,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6BD57F-E798-4F5D-A40D-A65A808483B8}">
-  <dimension ref="A1:BS36"/>
+  <dimension ref="A1:BV44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BQ17" sqref="BQ17:BQ21"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BW10" sqref="BW10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6263,7 +7267,7 @@
     <col min="9" max="9" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" s="4" customFormat="1">
+    <row r="1" spans="1:74" s="4" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>59</v>
       </c>
@@ -6341,7 +7345,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:71" s="6" customFormat="1">
+    <row r="2" spans="1:74" s="6" customFormat="1">
       <c r="A2" s="12" t="s">
         <v>28</v>
       </c>
@@ -6539,8 +7543,11 @@
       <c r="BS2" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:71" s="4" customFormat="1">
+      <c r="BU2" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:74" s="4" customFormat="1">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -6738,8 +7745,16 @@
         <f t="shared" si="0"/>
         <v>3.5520660333333336E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:71" s="6" customFormat="1">
+      <c r="BU3" s="4">
+        <f t="shared" ref="BU3:BV30" si="1">0.0145*BP3 - 0.2126</f>
+        <v>0.86657964074000005</v>
+      </c>
+      <c r="BV3" s="4">
+        <f>0.0145*BQ3 - 0.2126</f>
+        <v>0.55844154143999991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:74" s="6" customFormat="1">
       <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
@@ -6922,7 +7937,7 @@
         <v>1</v>
       </c>
       <c r="BP4" s="4">
-        <f t="shared" ref="BP4:BP7" si="1">AVERAGE(B4,M4,X4,AI4,AT5,BE4)</f>
+        <f t="shared" ref="BP4:BP7" si="2">AVERAGE(B4,M4,X4,AI4,AT5,BE4)</f>
         <v>95.347874678333326</v>
       </c>
       <c r="BQ4" s="4">
@@ -6937,8 +7952,16 @@
         <f t="shared" si="0"/>
         <v>3.7747866166666665E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:71" s="4" customFormat="1">
+      <c r="BU4" s="4">
+        <f t="shared" si="1"/>
+        <v>1.1699441828358332</v>
+      </c>
+      <c r="BV4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.15553645346083339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:74" s="4" customFormat="1">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -7121,7 +8144,7 @@
         <v>2</v>
       </c>
       <c r="BP5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90.504866015000005</v>
       </c>
       <c r="BQ5" s="4">
@@ -7136,8 +8159,16 @@
         <f t="shared" si="0"/>
         <v>3.5708939666666668E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:71" s="6" customFormat="1">
+      <c r="BU5" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0997205572175002</v>
+      </c>
+      <c r="BV5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.12409169277833337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:74" s="6" customFormat="1">
       <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
@@ -7320,7 +8351,7 @@
         <v>3</v>
       </c>
       <c r="BP6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80.784310539999993</v>
       </c>
       <c r="BQ6" s="4">
@@ -7335,8 +8366,16 @@
         <f t="shared" si="0"/>
         <v>3.1748400666666662E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:71" s="4" customFormat="1">
+      <c r="BU6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.95877250282999993</v>
+      </c>
+      <c r="BV6" s="4">
+        <f t="shared" si="1"/>
+        <v>7.1656161569166654E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:74" s="4" customFormat="1">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
@@ -7519,7 +8558,7 @@
         <v>4</v>
       </c>
       <c r="BP7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67.794624978000002</v>
       </c>
       <c r="BQ7" s="4">
@@ -7534,8 +8573,16 @@
         <f t="shared" si="0"/>
         <v>2.7151690999999999E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:71" s="6" customFormat="1">
+      <c r="BU7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.77042206218100007</v>
+      </c>
+      <c r="BV7" s="4">
+        <f t="shared" si="1"/>
+        <v>9.7006984912000049E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:74" s="6" customFormat="1">
       <c r="A8" s="12">
         <v>215</v>
       </c>
@@ -7617,8 +8664,10 @@
       <c r="BO8" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:71" s="4" customFormat="1">
+      <c r="BU8" s="4"/>
+      <c r="BV8" s="4"/>
+    </row>
+    <row r="9" spans="1:74" s="4" customFormat="1">
       <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
@@ -7809,19 +8858,27 @@
         <v>48.202060703977651</v>
       </c>
       <c r="BQ9" s="4">
-        <f t="shared" ref="BQ4:BQ13" si="2">AVERAGE(C10,N10,Y10,AJ10,AU10,BF10)</f>
+        <f t="shared" ref="BQ9:BQ13" si="3">AVERAGE(C10,N10,Y10,AJ10,AU10,BF10)</f>
         <v>66.267198298233311</v>
       </c>
       <c r="BR9" s="4">
-        <f t="shared" ref="BR4:BR13" si="3">AVERAGE(D10,O10,Z10,AK10,AV10,BG10)</f>
+        <f t="shared" ref="BR9:BR13" si="4">AVERAGE(D10,O10,Z10,AK10,AV10,BG10)</f>
         <v>2723.9791666666665</v>
       </c>
       <c r="BS9" s="4">
-        <f t="shared" ref="BS4:BS13" si="4">AVERAGE(E10,P10,AA10,AL10,AW10,BH10)</f>
+        <f t="shared" ref="BS9:BS13" si="5">AVERAGE(E10,P10,AA10,AL10,AW10,BH10)</f>
         <v>2.2343671991154918E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:71" s="6" customFormat="1">
+      <c r="BU9" s="4">
+        <f t="shared" si="1"/>
+        <v>0.48632988020767598</v>
+      </c>
+      <c r="BV9" s="4">
+        <f t="shared" si="1"/>
+        <v>0.74827437532438301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:74" s="6" customFormat="1">
       <c r="A10" s="12" t="s">
         <v>0</v>
       </c>
@@ -8004,23 +9061,31 @@
         <v>1</v>
       </c>
       <c r="BP10" s="6">
-        <f t="shared" ref="BP4:BP13" si="5">AVERAGE(B11,M11,X11,AI11,AT11,BE11)</f>
+        <f t="shared" ref="BP10:BP13" si="6">AVERAGE(B11,M11,X11,AI11,AT11,BE11)</f>
         <v>74.208596095121223</v>
       </c>
       <c r="BQ10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26.320449097278583</v>
       </c>
       <c r="BR10" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2815.3125</v>
       </c>
       <c r="BS10" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1500426738046879E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:71" s="4" customFormat="1">
+      <c r="BU10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.86342464337925773</v>
+      </c>
+      <c r="BV10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16904651191053949</v>
+      </c>
+    </row>
+    <row r="11" spans="1:74" s="4" customFormat="1">
       <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
@@ -8203,23 +9268,31 @@
         <v>2</v>
       </c>
       <c r="BP11" s="4">
+        <f t="shared" si="6"/>
+        <v>70.712062505562912</v>
+      </c>
+      <c r="BQ11" s="4">
+        <f t="shared" si="3"/>
+        <v>23.904684290768984</v>
+      </c>
+      <c r="BR11" s="4">
+        <f t="shared" si="4"/>
+        <v>2723.9791666666665</v>
+      </c>
+      <c r="BS11" s="4">
         <f t="shared" si="5"/>
-        <v>70.712062505562912</v>
-      </c>
-      <c r="BQ11" s="4">
-        <f t="shared" si="2"/>
-        <v>23.904684290768984</v>
-      </c>
-      <c r="BR11" s="4">
-        <f t="shared" si="3"/>
-        <v>2723.9791666666665</v>
-      </c>
-      <c r="BS11" s="4">
-        <f t="shared" si="4"/>
         <v>3.1187472305956299E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:71" s="6" customFormat="1">
+      <c r="BU11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.81272490633066219</v>
+      </c>
+      <c r="BV11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13401792221615028</v>
+      </c>
+    </row>
+    <row r="12" spans="1:74" s="6" customFormat="1">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -8402,23 +9475,31 @@
         <v>3</v>
       </c>
       <c r="BP12" s="6">
+        <f t="shared" si="6"/>
+        <v>63.180655873432045</v>
+      </c>
+      <c r="BQ12" s="6">
+        <f t="shared" si="3"/>
+        <v>29.855919365346697</v>
+      </c>
+      <c r="BR12" s="6">
+        <f t="shared" si="4"/>
+        <v>2723.9791666666665</v>
+      </c>
+      <c r="BS12" s="6">
         <f t="shared" si="5"/>
-        <v>63.180655873432045</v>
-      </c>
-      <c r="BQ12" s="6">
-        <f t="shared" si="2"/>
-        <v>29.855919365346697</v>
-      </c>
-      <c r="BR12" s="6">
-        <f t="shared" si="3"/>
-        <v>2723.9791666666665</v>
-      </c>
-      <c r="BS12" s="6">
-        <f t="shared" si="4"/>
         <v>2.8050714851571169E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:71" s="4" customFormat="1">
+      <c r="BU12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.70351951016476466</v>
+      </c>
+      <c r="BV12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.22031083079752711</v>
+      </c>
+    </row>
+    <row r="13" spans="1:74" s="4" customFormat="1">
       <c r="A13" s="10" t="s">
         <v>3</v>
       </c>
@@ -8601,23 +9682,31 @@
         <v>4</v>
       </c>
       <c r="BP13" s="4">
+        <f t="shared" si="6"/>
+        <v>53.146133306819422</v>
+      </c>
+      <c r="BQ13" s="4">
+        <f t="shared" si="3"/>
+        <v>34.536223786286136</v>
+      </c>
+      <c r="BR13" s="4">
+        <f t="shared" si="4"/>
+        <v>2857.75</v>
+      </c>
+      <c r="BS13" s="4">
         <f t="shared" si="5"/>
-        <v>53.146133306819422</v>
-      </c>
-      <c r="BQ13" s="4">
-        <f t="shared" si="2"/>
-        <v>34.536223786286136</v>
-      </c>
-      <c r="BR13" s="4">
-        <f t="shared" si="3"/>
-        <v>2857.75</v>
-      </c>
-      <c r="BS13" s="4">
-        <f t="shared" si="4"/>
         <v>2.3365923364988002E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:71" s="6" customFormat="1">
+      <c r="BU13" s="4">
+        <f t="shared" si="1"/>
+        <v>0.55801893294888161</v>
+      </c>
+      <c r="BV13" s="4">
+        <f t="shared" si="1"/>
+        <v>0.28817524490114899</v>
+      </c>
+    </row>
+    <row r="14" spans="1:74" s="6" customFormat="1">
       <c r="A14" s="12" t="s">
         <v>4</v>
       </c>
@@ -8796,8 +9885,10 @@
         <v>0.17664036999999999</v>
       </c>
       <c r="BN14" s="9"/>
-    </row>
-    <row r="15" spans="1:71">
+      <c r="BU14" s="4"/>
+      <c r="BV14" s="4"/>
+    </row>
+    <row r="15" spans="1:74">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -8870,8 +9961,10 @@
       <c r="BQ15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="16" spans="1:71" s="8" customFormat="1">
+      <c r="BU15" s="4"/>
+      <c r="BV15" s="4"/>
+    </row>
+    <row r="16" spans="1:74" s="8" customFormat="1">
       <c r="A16" s="14" t="s">
         <v>79</v>
       </c>
@@ -8957,8 +10050,10 @@
       <c r="BS16" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:71" s="6" customFormat="1">
+      <c r="BU16" s="4"/>
+      <c r="BV16" s="4"/>
+    </row>
+    <row r="17" spans="1:74" s="6" customFormat="1">
       <c r="A17" s="12" t="s">
         <v>28</v>
       </c>
@@ -9149,23 +10244,31 @@
         <v>0</v>
       </c>
       <c r="BP17" s="6">
-        <f>AVERAGE(B18,M18,X18,AI18,AT19,BE18)</f>
+        <f t="shared" ref="BP17:BS20" si="7">AVERAGE(B18,M18,X18,AI18,AT19,BE18)</f>
         <v>260.33273061046685</v>
       </c>
       <c r="BQ17" s="6">
-        <f>AVERAGE(C18,N18,Y18,AJ18,AU19,BF18)</f>
+        <f t="shared" si="7"/>
         <v>200.17276190279131</v>
       </c>
       <c r="BR17" s="6">
-        <f>AVERAGE(D18,O18,Z18,AK18,AV19,BG18)</f>
+        <f t="shared" si="7"/>
         <v>2029.0208333333333</v>
       </c>
       <c r="BS17" s="6">
-        <f>AVERAGE(E18,P18,AA18,AL18,AW19,BH18)</f>
+        <f t="shared" si="7"/>
         <v>0.14282244999494054</v>
       </c>
-    </row>
-    <row r="18" spans="1:71" s="8" customFormat="1">
+      <c r="BU17" s="4">
+        <f t="shared" si="1"/>
+        <v>3.5622245938517696</v>
+      </c>
+      <c r="BV17" s="4">
+        <f t="shared" si="1"/>
+        <v>2.6899050475904738</v>
+      </c>
+    </row>
+    <row r="18" spans="1:74" s="8" customFormat="1">
       <c r="A18" s="14" t="s">
         <v>0</v>
       </c>
@@ -9350,23 +10453,31 @@
         <v>1</v>
       </c>
       <c r="BP18" s="8">
-        <f>AVERAGE(B19,M19,X19,AI19,AT20,BE19)</f>
+        <f t="shared" si="7"/>
         <v>92.02282837709231</v>
       </c>
       <c r="BQ18" s="8">
-        <f>AVERAGE(C19,N19,Y19,AJ19,AU20,BF19)</f>
+        <f t="shared" si="7"/>
         <v>29.948867212616431</v>
       </c>
       <c r="BR18" s="8">
-        <f>AVERAGE(D19,O19,Z19,AK19,AV20,BG19)</f>
+        <f t="shared" si="7"/>
         <v>2029.0208333333333</v>
       </c>
       <c r="BS18" s="8">
-        <f>AVERAGE(E19,P19,AA19,AL19,AW20,BH19)</f>
+        <f t="shared" si="7"/>
         <v>5.0975481498100765E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:71" s="6" customFormat="1">
+      <c r="BU18" s="4">
+        <f t="shared" si="1"/>
+        <v>1.1217310114678387</v>
+      </c>
+      <c r="BV18" s="4">
+        <f t="shared" si="1"/>
+        <v>0.22165857458293825</v>
+      </c>
+    </row>
+    <row r="19" spans="1:74" s="6" customFormat="1">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9551,23 +10662,31 @@
         <v>2</v>
       </c>
       <c r="BP19" s="6">
-        <f>AVERAGE(B20,M20,X20,AI20,AT21,BE20)</f>
+        <f t="shared" si="7"/>
         <v>87.016809968022883</v>
       </c>
       <c r="BQ19" s="6">
-        <f>AVERAGE(C20,N20,Y20,AJ20,AU21,BF20)</f>
+        <f t="shared" si="7"/>
         <v>28.192981393093319</v>
       </c>
       <c r="BR19" s="6">
-        <f>AVERAGE(D20,O20,Z20,AK20,AV21,BG20)</f>
+        <f t="shared" si="7"/>
         <v>2029.0208333333333</v>
       </c>
       <c r="BS19" s="6">
-        <f>AVERAGE(E20,P20,AA20,AL20,AW21,BH20)</f>
+        <f t="shared" si="7"/>
         <v>4.7895474759873748E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:71" s="8" customFormat="1">
+      <c r="BU19" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0491437445363321</v>
+      </c>
+      <c r="BV19" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19619823019985316</v>
+      </c>
+    </row>
+    <row r="20" spans="1:74" s="8" customFormat="1">
       <c r="A20" s="14" t="s">
         <v>2</v>
       </c>
@@ -9752,23 +10871,31 @@
         <v>3</v>
       </c>
       <c r="BP20" s="8">
-        <f>AVERAGE(B21,M21,X21,AI21,AT22,BE21)</f>
+        <f t="shared" si="7"/>
         <v>76.280069946700849</v>
       </c>
       <c r="BQ20" s="8">
-        <f>AVERAGE(C21,N21,Y21,AJ21,AU22,BF21)</f>
+        <f t="shared" si="7"/>
         <v>23.270215442772734</v>
       </c>
       <c r="BR20" s="8">
-        <f>AVERAGE(D21,O21,Z21,AK21,AV22,BG21)</f>
+        <f t="shared" si="7"/>
         <v>2029.0208333333333</v>
       </c>
       <c r="BS20" s="8">
-        <f>AVERAGE(E21,P21,AA21,AL21,AW22,BH21)</f>
+        <f t="shared" si="7"/>
         <v>4.2037554448909144E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:71" s="6" customFormat="1">
+      <c r="BU20" s="4">
+        <f t="shared" si="1"/>
+        <v>0.89346101422716229</v>
+      </c>
+      <c r="BV20" s="4">
+        <f t="shared" si="1"/>
+        <v>0.12481812392020464</v>
+      </c>
+    </row>
+    <row r="21" spans="1:74" s="6" customFormat="1">
       <c r="A21" s="12" t="s">
         <v>3</v>
       </c>
@@ -9957,19 +11084,27 @@
         <v>65.554548462709462</v>
       </c>
       <c r="BQ21" s="8">
-        <f t="shared" ref="BQ21:BS21" si="6">AVERAGE(C22,N22,Y22,AJ22,AU23,BF22)</f>
+        <f t="shared" ref="BQ21:BS21" si="8">AVERAGE(C22,N22,Y22,AJ22,AU23,BF22)</f>
         <v>21.603857199428219</v>
       </c>
       <c r="BR21" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2118.9499999999998</v>
       </c>
       <c r="BS21" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.5311968188453696E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:71" s="8" customFormat="1">
+      <c r="BU21" s="4">
+        <f t="shared" si="1"/>
+        <v>0.73794095270928728</v>
+      </c>
+      <c r="BV21" s="4">
+        <f t="shared" si="1"/>
+        <v>0.1006559293917092</v>
+      </c>
+    </row>
+    <row r="22" spans="1:74" s="8" customFormat="1">
       <c r="A22" s="14" t="s">
         <v>4</v>
       </c>
@@ -10150,8 +11285,10 @@
         <v>0.75462264999999995</v>
       </c>
       <c r="BN22" s="9"/>
-    </row>
-    <row r="23" spans="1:71" s="6" customFormat="1">
+      <c r="BU22" s="4"/>
+      <c r="BV22" s="4"/>
+    </row>
+    <row r="23" spans="1:74" s="6" customFormat="1">
       <c r="A23" s="12">
         <v>210</v>
       </c>
@@ -10230,8 +11367,10 @@
       <c r="BL23" s="12"/>
       <c r="BM23" s="12"/>
       <c r="BN23" s="9"/>
-    </row>
-    <row r="24" spans="1:71" s="8" customFormat="1">
+      <c r="BU23" s="4"/>
+      <c r="BV23" s="4"/>
+    </row>
+    <row r="24" spans="1:74" s="8" customFormat="1">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -10301,8 +11440,10 @@
       <c r="BO24" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:71" s="6" customFormat="1">
+      <c r="BU24" s="4"/>
+      <c r="BV24" s="4"/>
+    </row>
+    <row r="25" spans="1:74" s="6" customFormat="1">
       <c r="A25" s="12" t="s">
         <v>34</v>
       </c>
@@ -10497,19 +11638,27 @@
         <v>266.48080051621997</v>
       </c>
       <c r="BQ25" s="6">
-        <f t="shared" ref="BQ18:BQ28" si="7">AVERAGE(C26,N26,Y26,AJ26,AU26,BF26)</f>
+        <f t="shared" ref="BQ25:BQ28" si="9">AVERAGE(C26,N26,Y26,AJ26,AU26,BF26)</f>
         <v>169.74576474014106</v>
       </c>
       <c r="BR25" s="6">
-        <f t="shared" ref="BR25:BR29" si="8">AVERAGE(D26,O26,Z26,AK26,AV26,BG26)</f>
+        <f t="shared" ref="BR25:BR29" si="10">AVERAGE(D26,O26,Z26,AK26,AV26,BG26)</f>
         <v>2074.4375</v>
       </c>
       <c r="BS25" s="6">
-        <f t="shared" ref="BS18:BS29" si="9">AVERAGE(E26,P26,AA26,AL26,AW26,BH26)</f>
+        <f t="shared" ref="BS25:BS29" si="11">AVERAGE(E26,P26,AA26,AL26,AW26,BH26)</f>
         <v>0.15898107926673014</v>
       </c>
-    </row>
-    <row r="26" spans="1:71" s="8" customFormat="1">
+      <c r="BU25" s="4">
+        <f t="shared" si="1"/>
+        <v>3.6513716074851899</v>
+      </c>
+      <c r="BV25" s="4">
+        <f t="shared" si="1"/>
+        <v>2.2487135887320453</v>
+      </c>
+    </row>
+    <row r="26" spans="1:74" s="8" customFormat="1">
       <c r="A26" s="14" t="s">
         <v>0</v>
       </c>
@@ -10698,19 +11847,27 @@
         <v>71.493343392241286</v>
       </c>
       <c r="BQ26" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>27.873753111756233</v>
       </c>
       <c r="BR26" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2055.75</v>
       </c>
       <c r="BS26" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.9528386164440495E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:71" s="6" customFormat="1">
+      <c r="BU26" s="4">
+        <f t="shared" si="1"/>
+        <v>0.82405347918749861</v>
+      </c>
+      <c r="BV26" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19156942012046541</v>
+      </c>
+    </row>
+    <row r="27" spans="1:74" s="6" customFormat="1">
       <c r="A27" s="12" t="s">
         <v>1</v>
       </c>
@@ -10899,19 +12056,27 @@
         <v>72.626107334051383</v>
       </c>
       <c r="BQ27" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>23.90611436455578</v>
       </c>
       <c r="BR27" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2074.4375</v>
       </c>
       <c r="BS27" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.9803878296599267E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:71" s="8" customFormat="1">
+      <c r="BU27" s="4">
+        <f t="shared" si="1"/>
+        <v>0.84047855634374502</v>
+      </c>
+      <c r="BV27" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13403865828605882</v>
+      </c>
+    </row>
+    <row r="28" spans="1:74" s="8" customFormat="1">
       <c r="A28" s="14" t="s">
         <v>2</v>
       </c>
@@ -11100,19 +12265,27 @@
         <v>63.612485621052606</v>
       </c>
       <c r="BQ28" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>20.334536847693684</v>
       </c>
       <c r="BR28" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2074.4375</v>
       </c>
       <c r="BS28" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.4977657601842897E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:71" s="6" customFormat="1">
+      <c r="BU28" s="4">
+        <f t="shared" si="1"/>
+        <v>0.70978104150526278</v>
+      </c>
+      <c r="BV28" s="4">
+        <f t="shared" si="1"/>
+        <v>8.225078429155841E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:74" s="6" customFormat="1">
       <c r="A29" s="12" t="s">
         <v>3</v>
       </c>
@@ -11301,19 +12474,27 @@
         <v>57.302363010918818</v>
       </c>
       <c r="BQ29" s="6">
-        <f t="shared" ref="BQ29" si="10">AVERAGE(C30,N30,Y30,AJ30,AU30,BF30)</f>
+        <f t="shared" ref="BQ29" si="12">AVERAGE(C30,N30,Y30,AJ30,AU30,BF30)</f>
         <v>19.405117775936439</v>
       </c>
       <c r="BR29" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2210.8000000000002</v>
       </c>
       <c r="BS29" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2.9920470684951756E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:71" s="8" customFormat="1">
+      <c r="BU29" s="4">
+        <f t="shared" si="1"/>
+        <v>0.6182842636583229</v>
+      </c>
+      <c r="BV29" s="4">
+        <f t="shared" si="1"/>
+        <v>6.8774207751078398E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:74" s="8" customFormat="1">
       <c r="A30" s="14" t="s">
         <v>4</v>
       </c>
@@ -11494,8 +12675,10 @@
         <v>0.199250235008436</v>
       </c>
       <c r="BN30" s="9"/>
-    </row>
-    <row r="31" spans="1:71">
+      <c r="BU30" s="4"/>
+      <c r="BV30" s="4"/>
+    </row>
+    <row r="31" spans="1:74">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -11556,7 +12739,7 @@
       <c r="BF31" s="9"/>
       <c r="BG31" s="9"/>
     </row>
-    <row r="34" spans="2:27">
+    <row r="34" spans="2:50">
       <c r="B34" s="14">
         <v>26.00896389</v>
       </c>
@@ -11583,14 +12766,60 @@
       <c r="Z34" s="12"/>
       <c r="AA34" s="12"/>
     </row>
-    <row r="36" spans="2:27">
+    <row r="36" spans="2:50">
       <c r="Q36" s="14"/>
       <c r="R36" s="14"/>
       <c r="S36" s="14"/>
       <c r="T36" s="14"/>
       <c r="V36" s="14"/>
     </row>
+    <row r="39" spans="2:50">
+      <c r="AV39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="2:50">
+      <c r="AW40" t="s">
+        <v>88</v>
+      </c>
+      <c r="AX40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="2:50">
+      <c r="AW41" s="6">
+        <v>83.39</v>
+      </c>
+      <c r="AX41" s="4">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="42" spans="2:50">
+      <c r="AW42" s="6">
+        <v>215.78</v>
+      </c>
+      <c r="AX42" s="4">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="43" spans="2:50">
+      <c r="AW43" s="6">
+        <v>360.4</v>
+      </c>
+      <c r="AX43" s="4">
+        <v>5.24</v>
+      </c>
+    </row>
+    <row r="44" spans="2:50">
+      <c r="AW44" s="6">
+        <v>521.98</v>
+      </c>
+      <c r="AX44" s="4">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>